<commit_message>
updated excel and req
</commit_message>
<xml_diff>
--- a/dday.xlsx
+++ b/dday.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\3D Objects\display\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8315E78D-FCF0-4A4F-91A8-5AD4A650D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ward</t>
   </si>
@@ -44,43 +50,13 @@
   </si>
   <si>
     <t>major</t>
-  </si>
-  <si>
-    <t>hon_Farah</t>
-  </si>
-  <si>
-    <t>kheyrow</t>
-  </si>
-  <si>
-    <t>a_Issack</t>
-  </si>
-  <si>
-    <t>IFTIN</t>
-  </si>
-  <si>
-    <t>WABERI</t>
-  </si>
-  <si>
-    <t>GALBET</t>
-  </si>
-  <si>
-    <t>COUNTY HIGH SCHOOL:1</t>
-  </si>
-  <si>
-    <t>GARISSA PRIMARY SCHOOL:1</t>
-  </si>
-  <si>
-    <t>GARISSA SECONDARY SCHOOL:1</t>
-  </si>
-  <si>
-    <t>JAMUHURI CLUB:1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +119,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +205,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +257,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,14 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,207 +493,9 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>450</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>200</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>50</v>
-      </c>
-      <c r="J2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>1520</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1100</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>400</v>
-      </c>
-      <c r="I3">
-        <v>600</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>1520</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1100</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>400</v>
-      </c>
-      <c r="I4">
-        <v>600</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>1520</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1100</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>400</v>
-      </c>
-      <c r="I5">
-        <v>600</v>
-      </c>
-      <c r="J5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>453</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>253</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>101</v>
-      </c>
-      <c r="I6">
-        <v>101</v>
-      </c>
-      <c r="J6">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>450</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>250</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
-      </c>
-      <c r="I7">
-        <v>100</v>
-      </c>
-      <c r="J7">
-        <v>50</v>
-      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>